<commit_message>
Testing bound box intersections by multiplying by a ray's inverse direction as opposed to dividing by its direction gave a significant performance boost.
</commit_message>
<xml_diff>
--- a/Statistics/BVH_Performance.xlsx
+++ b/Statistics/BVH_Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Projects\Radiance\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6964DD7-A46D-4BC0-A1FF-66AFA28DEA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD2ACC9-8ACC-4520-9B35-94BF3E93B07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A5432B80-60C3-4BA9-AB2E-A1ED8FBAF94F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
   <si>
     <t>SAH v1</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>SAH v1 closest child v2</t>
+  </si>
+  <si>
+    <t>Ray inv_d</t>
   </si>
 </sst>
 </file>
@@ -8754,6 +8757,777 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-568A-4968-970B-927AA61AD5DE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'unity.tri 2'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ray inv_d</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'unity.tri 2'!$A$2:$A$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="120"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'unity.tri 2'!$F$2:$F$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="120"/>
+                <c:pt idx="0">
+                  <c:v>528.06899999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>538.94899999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>567.41600000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>553.78099999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>587.61300000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>652.47699999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>632.83399999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>606.66600000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>589.85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>578.11400000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>573.48199999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>559.05600000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>540.37300000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>533.69500000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>515.96199999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>500.13200000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>492.33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>485.995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>472.61500000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>452.03500000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>458.17200000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>468.72699999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>471.55900000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>492.36</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>481.911</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>476.21100000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>475.48500000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>482.66199999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>482.16399999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>477.58</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>477.858</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>474.863</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>459.52699999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>451.512</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>438.42200000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>428.38200000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>428.38</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>426.375</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>431.05099999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>439.726</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>451.89800000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>457.99900000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>470.005</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>486.56</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>499.96499999999997</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>506.99099999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>522.86300000000006</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>539.98099999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>556.09699999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>571.89300000000003</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>595.30999999999995</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>613.72500000000002</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>636.21299999999997</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>660.096</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>681.01900000000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>699.97799999999995</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>728.02499999999998</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>742.68299999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>764.84199999999998</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>772.66300000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>775.84799999999996</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>799.92100000000005</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>800.46900000000005</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>808.26400000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>807.721</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>808.447</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>823.94</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>824.38800000000003</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>836.654</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>856.50800000000004</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>867.697</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>887.75</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>910.96799999999996</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>918.899</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>936.46699999999998</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>947.01499999999999</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>961.49699999999996</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>977.01900000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1009.35</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1024.27</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1032.45</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1072.8499999999999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1079.8900000000001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1097.24</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1129.3599999999999</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1138.76</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1159.3499999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1182.25</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1208.82</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1202.03</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1208.23</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1222.97</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1223.92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1214.77</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1196.49</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1159.57</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1159.54</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1115.45</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1095.8399999999999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1080.4100000000001</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1044.48</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1022.3</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>991.11900000000003</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>958.63400000000001</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>941.14</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>915.19899999999996</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>930.09900000000005</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>884.29700000000003</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>861.24300000000005</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>852.37</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>836.99199999999996</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>826.524</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>811.93899999999996</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>790.96699999999998</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>783.83299999999997</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>773.78</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>762.125</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>743.91899999999998</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>738.30200000000002</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>720.69200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4AE2-4699-8D04-E7775DBBE84B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -23137,13 +23911,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -27077,10 +27851,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1F2289-1ADE-4875-A98C-2E60B5E7C362}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27090,9 +27864,10 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -27108,8 +27883,11 @@
       <c r="E1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -27125,8 +27903,11 @@
       <c r="E2">
         <v>343.983</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>528.06899999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -27142,8 +27923,11 @@
       <c r="E3">
         <v>335.96499999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>538.94899999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -27159,8 +27943,11 @@
       <c r="E4">
         <v>330.59500000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>567.41600000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -27176,8 +27963,11 @@
       <c r="E5">
         <v>323.77600000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>553.78099999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -27193,8 +27983,11 @@
       <c r="E6">
         <v>317.19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>587.61300000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -27210,8 +28003,11 @@
       <c r="E7">
         <v>310.70400000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>652.47699999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -27227,8 +28023,11 @@
       <c r="E8">
         <v>302.58800000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>632.83399999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -27244,8 +28043,11 @@
       <c r="E9">
         <v>299.06599999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>606.66600000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -27261,8 +28063,11 @@
       <c r="E10">
         <v>385.79500000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>589.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -27278,8 +28083,11 @@
       <c r="E11">
         <v>372.096</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>578.11400000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -27295,8 +28103,11 @@
       <c r="E12">
         <v>368.726</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>573.48199999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -27312,8 +28123,11 @@
       <c r="E13">
         <v>360.35500000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>559.05600000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -27329,8 +28143,11 @@
       <c r="E14">
         <v>348.61099999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>540.37300000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -27346,8 +28163,11 @@
       <c r="E15">
         <v>341.64299999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>533.69500000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -27363,8 +28183,11 @@
       <c r="E16">
         <v>331.57400000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>515.96199999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -27380,8 +28203,11 @@
       <c r="E17">
         <v>320.39100000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>500.13200000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -27397,8 +28223,11 @@
       <c r="E18">
         <v>317.06099999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>492.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -27414,8 +28243,11 @@
       <c r="E19">
         <v>309.88799999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>485.995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -27431,8 +28263,11 @@
       <c r="E20">
         <v>306.15699999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>472.61500000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -27448,8 +28283,11 @@
       <c r="E21">
         <v>303.48099999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>452.03500000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -27465,8 +28303,11 @@
       <c r="E22">
         <v>301.81200000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>458.17200000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -27482,8 +28323,11 @@
       <c r="E23">
         <v>299.92099999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>468.72699999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -27499,8 +28343,11 @@
       <c r="E24">
         <v>299.072</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>471.55900000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -27516,8 +28363,11 @@
       <c r="E25">
         <v>308.39400000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>492.36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -27533,8 +28383,11 @@
       <c r="E26">
         <v>306.81099999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>481.911</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -27550,8 +28403,11 @@
       <c r="E27">
         <v>301.08800000000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>476.21100000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -27567,8 +28423,11 @@
       <c r="E28">
         <v>302.19200000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <v>475.48500000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -27584,8 +28443,11 @@
       <c r="E29">
         <v>302.63600000000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <v>482.66199999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -27601,8 +28463,11 @@
       <c r="E30">
         <v>298.81799999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <v>482.16399999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -27618,8 +28483,11 @@
       <c r="E31">
         <v>297.81</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <v>477.58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -27635,8 +28503,11 @@
       <c r="E32">
         <v>298.68700000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <v>477.858</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -27652,8 +28523,11 @@
       <c r="E33">
         <v>297.70299999999997</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <v>474.863</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -27669,8 +28543,11 @@
       <c r="E34">
         <v>295.41300000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <v>459.52699999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -27686,8 +28563,11 @@
       <c r="E35">
         <v>287.59199999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>451.512</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -27703,8 +28583,11 @@
       <c r="E36">
         <v>267.91500000000002</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <v>438.42200000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -27720,8 +28603,11 @@
       <c r="E37">
         <v>261.13</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <v>428.38200000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -27737,8 +28623,11 @@
       <c r="E38">
         <v>262.25299999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <v>428.38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -27754,8 +28643,11 @@
       <c r="E39">
         <v>264.52600000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <v>426.375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -27771,8 +28663,11 @@
       <c r="E40">
         <v>269.93799999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <v>431.05099999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -27788,8 +28683,11 @@
       <c r="E41">
         <v>275.36399999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <v>439.726</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -27805,8 +28703,11 @@
       <c r="E42">
         <v>280.62700000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <v>451.89800000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -27822,8 +28723,11 @@
       <c r="E43">
         <v>289.58</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <v>457.99900000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -27839,8 +28743,11 @@
       <c r="E44">
         <v>299.79000000000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <v>470.005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -27856,8 +28763,11 @@
       <c r="E45">
         <v>311.29300000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <v>486.56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -27873,8 +28783,11 @@
       <c r="E46">
         <v>319.50299999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <v>499.96499999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -27890,8 +28803,11 @@
       <c r="E47">
         <v>329.452</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>506.99099999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -27907,8 +28823,11 @@
       <c r="E48">
         <v>341.40499999999997</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <v>522.86300000000006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -27924,8 +28843,11 @@
       <c r="E49">
         <v>354.55399999999997</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <v>539.98099999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -27941,8 +28863,11 @@
       <c r="E50">
         <v>365.709</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50">
+        <v>556.09699999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -27958,8 +28883,11 @@
       <c r="E51">
         <v>375.68400000000003</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <v>571.89300000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -27975,8 +28903,11 @@
       <c r="E52">
         <v>385.34399999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <v>595.30999999999995</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -27992,8 +28923,11 @@
       <c r="E53">
         <v>399.40800000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <v>613.72500000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -28009,8 +28943,11 @@
       <c r="E54">
         <v>418.00799999999998</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <v>636.21299999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -28026,8 +28963,11 @@
       <c r="E55">
         <v>426.685</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <v>660.096</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -28043,8 +28983,11 @@
       <c r="E56">
         <v>447.863</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56">
+        <v>681.01900000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -28060,8 +29003,11 @@
       <c r="E57">
         <v>460.16199999999998</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57">
+        <v>699.97799999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -28077,8 +29023,11 @@
       <c r="E58">
         <v>478.69</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <v>728.02499999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -28094,8 +29043,11 @@
       <c r="E59">
         <v>492.77499999999998</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <v>742.68299999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -28111,8 +29063,11 @@
       <c r="E60">
         <v>500.69499999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60">
+        <v>764.84199999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -28128,8 +29083,11 @@
       <c r="E61">
         <v>510.29599999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61">
+        <v>772.66300000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -28145,8 +29103,11 @@
       <c r="E62">
         <v>517.13800000000003</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62">
+        <v>775.84799999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -28162,8 +29123,11 @@
       <c r="E63">
         <v>521.94100000000003</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63">
+        <v>799.92100000000005</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -28179,8 +29143,11 @@
       <c r="E64">
         <v>530.38199999999995</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <v>800.46900000000005</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -28196,8 +29163,11 @@
       <c r="E65">
         <v>534.09900000000005</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65">
+        <v>808.26400000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -28213,8 +29183,11 @@
       <c r="E66">
         <v>542.46799999999996</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66">
+        <v>807.721</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -28230,8 +29203,11 @@
       <c r="E67">
         <v>550.38</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67">
+        <v>808.447</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -28247,8 +29223,11 @@
       <c r="E68">
         <v>549.39200000000005</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <v>823.94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -28264,8 +29243,11 @@
       <c r="E69">
         <v>553.96</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <v>824.38800000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -28281,8 +29263,11 @@
       <c r="E70">
         <v>559.15800000000002</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70">
+        <v>836.654</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -28298,8 +29283,11 @@
       <c r="E71">
         <v>561.41499999999996</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71">
+        <v>856.50800000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -28315,8 +29303,11 @@
       <c r="E72">
         <v>573.78200000000004</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72">
+        <v>867.697</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -28332,8 +29323,11 @@
       <c r="E73">
         <v>588.31600000000003</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <v>887.75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -28349,8 +29343,11 @@
       <c r="E74">
         <v>591.81500000000005</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <v>910.96799999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -28366,8 +29363,11 @@
       <c r="E75">
         <v>612.16899999999998</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <v>918.899</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -28383,8 +29383,11 @@
       <c r="E76">
         <v>623.13900000000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <v>936.46699999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -28400,8 +29403,11 @@
       <c r="E77">
         <v>622.75099999999998</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <v>947.01499999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -28417,8 +29423,11 @@
       <c r="E78">
         <v>640.56700000000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78">
+        <v>961.49699999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -28434,8 +29443,11 @@
       <c r="E79">
         <v>655.44</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <v>977.01900000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -28451,8 +29463,11 @@
       <c r="E80">
         <v>661.77599999999995</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <v>1009.35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -28468,8 +29483,11 @@
       <c r="E81">
         <v>682.60799999999995</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <v>1024.27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -28485,8 +29503,11 @@
       <c r="E82">
         <v>698.03499999999997</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <v>1032.45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -28502,8 +29523,11 @@
       <c r="E83">
         <v>716.88800000000003</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <v>1072.8499999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -28519,8 +29543,11 @@
       <c r="E84">
         <v>724.89499999999998</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84">
+        <v>1079.8900000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -28536,8 +29563,11 @@
       <c r="E85">
         <v>733.90599999999995</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85">
+        <v>1097.24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -28553,8 +29583,11 @@
       <c r="E86">
         <v>751.40200000000004</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86">
+        <v>1129.3599999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -28570,8 +29603,11 @@
       <c r="E87">
         <v>751.029</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87">
+        <v>1138.76</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -28587,8 +29623,11 @@
       <c r="E88">
         <v>768.68399999999997</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88">
+        <v>1159.3499999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -28604,8 +29643,11 @@
       <c r="E89">
         <v>789.51599999999996</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89">
+        <v>1182.25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -28621,8 +29663,11 @@
       <c r="E90">
         <v>800.79700000000003</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90">
+        <v>1208.82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -28638,8 +29683,11 @@
       <c r="E91">
         <v>808.17399999999998</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91">
+        <v>1202.03</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -28655,8 +29703,11 @@
       <c r="E92">
         <v>806.24400000000003</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92">
+        <v>1208.23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -28672,8 +29723,11 @@
       <c r="E93">
         <v>824.01199999999994</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93">
+        <v>1222.97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -28689,8 +29743,11 @@
       <c r="E94">
         <v>812.61300000000006</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94">
+        <v>1223.92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -28706,8 +29763,11 @@
       <c r="E95">
         <v>824.38</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95">
+        <v>1214.77</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -28723,8 +29783,11 @@
       <c r="E96">
         <v>815.39200000000005</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96">
+        <v>1196.49</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -28740,8 +29803,11 @@
       <c r="E97">
         <v>792.73699999999997</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97">
+        <v>1159.57</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -28757,8 +29823,11 @@
       <c r="E98">
         <v>782.90200000000004</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98">
+        <v>1159.54</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -28774,8 +29843,11 @@
       <c r="E99">
         <v>758.46199999999999</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99">
+        <v>1115.45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -28791,8 +29863,11 @@
       <c r="E100">
         <v>742.52599999999995</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100">
+        <v>1095.8399999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -28808,8 +29883,11 @@
       <c r="E101">
         <v>725.11900000000003</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101">
+        <v>1080.4100000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -28825,8 +29903,11 @@
       <c r="E102">
         <v>708.45799999999997</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102">
+        <v>1044.48</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -28842,8 +29923,11 @@
       <c r="E103">
         <v>686.25400000000002</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F103">
+        <v>1022.3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -28859,8 +29943,11 @@
       <c r="E104">
         <v>670.65700000000004</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F104">
+        <v>991.11900000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -28876,8 +29963,11 @@
       <c r="E105">
         <v>657.30899999999997</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F105">
+        <v>958.63400000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -28893,8 +29983,11 @@
       <c r="E106">
         <v>640.81899999999996</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F106">
+        <v>941.14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -28910,8 +30003,11 @@
       <c r="E107">
         <v>619.923</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F107">
+        <v>915.19899999999996</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -28927,8 +30023,11 @@
       <c r="E108">
         <v>604.67100000000005</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F108">
+        <v>930.09900000000005</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -28944,8 +30043,11 @@
       <c r="E109">
         <v>584.41499999999996</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F109">
+        <v>884.29700000000003</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -28961,8 +30063,11 @@
       <c r="E110">
         <v>578.61900000000003</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F110">
+        <v>861.24300000000005</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -28978,8 +30083,11 @@
       <c r="E111">
         <v>568.34100000000001</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F111">
+        <v>852.37</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -28995,8 +30103,11 @@
       <c r="E112">
         <v>556.37199999999996</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F112">
+        <v>836.99199999999996</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -29012,8 +30123,11 @@
       <c r="E113">
         <v>544.66899999999998</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F113">
+        <v>826.524</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -29029,8 +30143,11 @@
       <c r="E114">
         <v>536.34799999999996</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F114">
+        <v>811.93899999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -29046,8 +30163,11 @@
       <c r="E115">
         <v>532.28399999999999</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F115">
+        <v>790.96699999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -29063,8 +30183,11 @@
       <c r="E116">
         <v>525.68799999999999</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F116">
+        <v>783.83299999999997</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -29080,8 +30203,11 @@
       <c r="E117">
         <v>512.84199999999998</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F117">
+        <v>773.78</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -29097,8 +30223,11 @@
       <c r="E118">
         <v>502.34</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F118">
+        <v>762.125</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -29114,8 +30243,11 @@
       <c r="E119">
         <v>485.74299999999999</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F119">
+        <v>743.91899999999998</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -29131,8 +30263,11 @@
       <c r="E120">
         <v>483.19</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F120">
+        <v>738.30200000000002</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -29147,6 +30282,9 @@
       </c>
       <c r="E121">
         <v>474.78</v>
+      </c>
+      <c r="F121">
+        <v>720.69200000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started work on improving the build time for the BVH.
</commit_message>
<xml_diff>
--- a/Statistics/BVH_Performance.xlsx
+++ b/Statistics/BVH_Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Projects\Radiance\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9C0B52-B0CE-4F2F-A3C5-51023D3F97D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B49FA2F-2C4E-4E88-9107-3E3217E94036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{A5432B80-60C3-4BA9-AB2E-A1ED8FBAF94F}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t>SAH v1</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>WL 2 SPP SbP offset</t>
+  </si>
+  <si>
+    <t>Binned BVH</t>
   </si>
 </sst>
 </file>
@@ -20272,6 +20275,779 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-C140-4A67-9C47-B4EB34F08BDB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'unity.tri 3 MSPS'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Binned BVH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'unity.tri 3 MSPS'!$A$2:$A$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="120"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'unity.tri 3 MSPS'!$K$2:$K$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="120"/>
+                <c:pt idx="0">
+                  <c:v>1783.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1546.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1595.66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1508.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1313.56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1296.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1386.49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1413.03</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1358.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1295.79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1267.1300000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1267.08</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1226.54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1153.18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1163.01</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1111.24</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1093.06</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1076.33</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1072.9000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1041.58</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1044.02</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1042.27</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1039.81</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1049.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1039.07</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1032.21</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1029.44</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1017.08</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1009.05</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1000.89</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1007.37</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>992.13900000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>989.73699999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>973.375</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>952.05899999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>943.625</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>940.07399999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>942.65</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>950.74</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>946.47900000000004</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>991.07</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1024.23</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1044.48</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1086.74</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1132</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1164.08</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1227.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1277.1400000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1244.8499999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1327.86</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1420.68</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1442.92</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1502.37</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1546.21</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1575.34</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1582.15</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1622.02</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1709.43</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1695.72</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1714.99</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1801.51</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1853.05</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1833.17</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1845.29</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1886.25</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1928.2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1970.15</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2000.75</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2022.62</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2050.2600000000002</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2106.89</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2159.86</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2180.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2210.5100000000002</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2256</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2305.25</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2336.1799999999998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2393.27</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2439.0500000000002</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2494.17</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2528.19</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2545.52</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2589.48</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2654.03</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2710.52</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2744.29</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2727.21</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2747.07</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2787.43</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2814.13</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2832.07</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2845.69</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2839.33</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2783.28</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2746.08</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2729.64</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2691.61</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2640.92</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2559.92</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2491.91</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2445.04</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2388.0500000000002</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2301.31</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2248.7199999999998</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2143.19</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2012.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1892.85</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1822.47</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1863.41</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1877.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1841.11</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1763.71</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1698.81</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1684.9</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1655.23</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1619.13</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1586.02</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1564.88</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1536.53</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1548.89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E83C-41A1-A7BB-93C155C1481B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -42237,13 +43013,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>563880</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
@@ -48705,10 +49481,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8750E5EE-F956-401B-AB0D-294E07FBDD80}">
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48725,7 +49501,7 @@
     <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -48756,8 +49532,11 @@
       <c r="J1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -48788,8 +49567,11 @@
       <c r="J2">
         <v>1945.73</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>1783.91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -48820,8 +49602,11 @@
       <c r="J3">
         <v>1875.27</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>1546.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -48852,8 +49637,11 @@
       <c r="J4">
         <v>1917.86</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>1595.66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -48884,8 +49672,11 @@
       <c r="J5">
         <v>1873.67</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>1508.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -48916,8 +49707,11 @@
       <c r="J6">
         <v>1839.93</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>1313.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -48948,8 +49742,11 @@
       <c r="J7">
         <v>1789.54</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>1296.71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -48980,8 +49777,11 @@
       <c r="J8">
         <v>1702.05</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>1386.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -49012,8 +49812,11 @@
       <c r="J9">
         <v>1616.36</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>1413.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -49044,8 +49847,11 @@
       <c r="J10">
         <v>1605.47</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>1358.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -49076,8 +49882,11 @@
       <c r="J11">
         <v>1572.68</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>1295.79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -49108,8 +49917,11 @@
       <c r="J12">
         <v>1547.86</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>1267.1300000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -49140,8 +49952,11 @@
       <c r="J13">
         <v>1513.99</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <v>1267.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -49172,8 +49987,11 @@
       <c r="J14">
         <v>1472.55</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <v>1226.54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -49204,8 +50022,11 @@
       <c r="J15">
         <v>1430.18</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <v>1153.18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -49236,8 +50057,11 @@
       <c r="J16">
         <v>1401.94</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>1163.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -49268,8 +50092,11 @@
       <c r="J17">
         <v>1364.04</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>1111.24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -49300,8 +50127,11 @@
       <c r="J18">
         <v>1333.52</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>1093.06</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -49332,8 +50162,11 @@
       <c r="J19">
         <v>1307.3900000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>1076.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -49364,8 +50197,11 @@
       <c r="J20">
         <v>1285.26</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>1072.9000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -49396,8 +50232,11 @@
       <c r="J21">
         <v>1266.4000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>1041.58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -49428,8 +50267,11 @@
       <c r="J22">
         <v>1242.3399999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>1044.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -49460,8 +50302,11 @@
       <c r="J23">
         <v>1241.49</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>1042.27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -49492,8 +50337,11 @@
       <c r="J24">
         <v>1252.19</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>1039.81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -49524,8 +50372,11 @@
       <c r="J25">
         <v>1265.18</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>1049.23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -49556,8 +50407,11 @@
       <c r="J26">
         <v>1252</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>1039.07</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -49588,8 +50442,11 @@
       <c r="J27">
         <v>1241.43</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>1032.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -49620,8 +50477,11 @@
       <c r="J28">
         <v>1234.07</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>1029.44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -49652,8 +50512,11 @@
       <c r="J29">
         <v>1229.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>1017.08</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -49684,8 +50547,11 @@
       <c r="J30">
         <v>1220.08</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30">
+        <v>1009.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -49716,8 +50582,11 @@
       <c r="J31">
         <v>1211.28</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <v>1000.89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -49748,8 +50617,11 @@
       <c r="J32">
         <v>1206.33</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>1007.37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -49780,8 +50652,11 @@
       <c r="J33">
         <v>1196.6199999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <v>992.13900000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -49812,8 +50687,11 @@
       <c r="J34">
         <v>1189.08</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34">
+        <v>989.73699999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -49844,8 +50722,11 @@
       <c r="J35">
         <v>1172.0999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>973.375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -49876,8 +50757,11 @@
       <c r="J36">
         <v>1149.94</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <v>952.05899999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -49908,8 +50792,11 @@
       <c r="J37">
         <v>1130.94</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>943.625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -49940,8 +50827,11 @@
       <c r="J38">
         <v>1123.24</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>940.07399999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -49972,8 +50862,11 @@
       <c r="J39">
         <v>1124.17</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>942.65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -50004,8 +50897,11 @@
       <c r="J40">
         <v>1136.19</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K40">
+        <v>950.74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -50036,8 +50932,11 @@
       <c r="J41">
         <v>1153.53</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K41">
+        <v>946.47900000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -50068,8 +50967,11 @@
       <c r="J42">
         <v>1182.01</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K42">
+        <v>991.07</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -50100,8 +51002,11 @@
       <c r="J43">
         <v>1214.2</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K43">
+        <v>1024.23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -50132,8 +51037,11 @@
       <c r="J44">
         <v>1255.05</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K44">
+        <v>1044.48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -50164,8 +51072,11 @@
       <c r="J45">
         <v>1299.32</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K45">
+        <v>1086.74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -50196,8 +51107,11 @@
       <c r="J46">
         <v>1347.62</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K46">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -50228,8 +51142,11 @@
       <c r="J47">
         <v>1389.01</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K47">
+        <v>1164.08</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -50260,8 +51177,11 @@
       <c r="J48">
         <v>1441.42</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K48">
+        <v>1227.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -50292,8 +51212,11 @@
       <c r="J49">
         <v>1490.68</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K49">
+        <v>1277.1400000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -50324,8 +51247,11 @@
       <c r="J50">
         <v>1535.82</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K50">
+        <v>1244.8499999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -50356,8 +51282,11 @@
       <c r="J51">
         <v>1578.18</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K51">
+        <v>1327.86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -50388,8 +51317,11 @@
       <c r="J52">
         <v>1630.26</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K52">
+        <v>1420.68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -50420,8 +51352,11 @@
       <c r="J53">
         <v>1691.41</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K53">
+        <v>1442.92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -50452,8 +51387,11 @@
       <c r="J54">
         <v>1765.65</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K54">
+        <v>1502.37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -50484,8 +51422,11 @@
       <c r="J55">
         <v>1838.95</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K55">
+        <v>1546.21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -50516,8 +51457,11 @@
       <c r="J56">
         <v>1890.45</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K56">
+        <v>1575.34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -50548,8 +51492,11 @@
       <c r="J57">
         <v>1951.43</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K57">
+        <v>1582.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -50580,8 +51527,11 @@
       <c r="J58">
         <v>2016.19</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K58">
+        <v>1622.02</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -50612,8 +51562,11 @@
       <c r="J59">
         <v>2067.35</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K59">
+        <v>1709.43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -50644,8 +51597,11 @@
       <c r="J60">
         <v>2130.77</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K60">
+        <v>1695.72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -50676,8 +51632,11 @@
       <c r="J61">
         <v>2168.4699999999998</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K61">
+        <v>1714.99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -50708,8 +51667,11 @@
       <c r="J62">
         <v>2200.35</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K62">
+        <v>1801.51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -50740,8 +51702,11 @@
       <c r="J63">
         <v>2228.36</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K63">
+        <v>1853.05</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -50772,8 +51737,11 @@
       <c r="J64">
         <v>2255.83</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K64">
+        <v>1833.17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -50804,8 +51772,11 @@
       <c r="J65">
         <v>2279.4899999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K65">
+        <v>1845.29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -50836,8 +51807,11 @@
       <c r="J66">
         <v>2296.84</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K66">
+        <v>1886.25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -50868,8 +51842,11 @@
       <c r="J67">
         <v>2339.19</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K67">
+        <v>1928.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -50900,8 +51877,11 @@
       <c r="J68">
         <v>2371.36</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K68">
+        <v>1970.15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -50932,8 +51912,11 @@
       <c r="J69">
         <v>2416.1999999999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K69">
+        <v>2000.75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -50964,8 +51947,11 @@
       <c r="J70">
         <v>2446.0700000000002</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K70">
+        <v>2022.62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -50996,8 +51982,11 @@
       <c r="J71">
         <v>2498.96</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K71">
+        <v>2050.2600000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -51028,8 +52017,11 @@
       <c r="J72">
         <v>2548.37</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K72">
+        <v>2106.89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -51060,8 +52052,11 @@
       <c r="J73">
         <v>2595.9499999999998</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K73">
+        <v>2159.86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -51092,8 +52087,11 @@
       <c r="J74">
         <v>2646.12</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K74">
+        <v>2180.8000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -51124,8 +52122,11 @@
       <c r="J75">
         <v>2683.45</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K75">
+        <v>2210.5100000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -51156,8 +52157,11 @@
       <c r="J76">
         <v>2730.15</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K76">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -51188,8 +52192,11 @@
       <c r="J77">
         <v>2764.07</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K77">
+        <v>2305.25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -51220,8 +52227,11 @@
       <c r="J78">
         <v>2801.47</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K78">
+        <v>2336.1799999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -51252,8 +52262,11 @@
       <c r="J79">
         <v>2854.2</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K79">
+        <v>2393.27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -51284,8 +52297,11 @@
       <c r="J80">
         <v>2897.57</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K80">
+        <v>2439.0500000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -51316,8 +52332,11 @@
       <c r="J81">
         <v>2957.33</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K81">
+        <v>2494.17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -51348,8 +52367,11 @@
       <c r="J82">
         <v>3008.22</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K82">
+        <v>2528.19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -51380,8 +52402,11 @@
       <c r="J83">
         <v>3066.62</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K83">
+        <v>2545.52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -51412,8 +52437,11 @@
       <c r="J84">
         <v>3111.72</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K84">
+        <v>2589.48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -51444,8 +52472,11 @@
       <c r="J85">
         <v>3162</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K85">
+        <v>2654.03</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -51476,8 +52507,11 @@
       <c r="J86">
         <v>3201.41</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K86">
+        <v>2710.52</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -51508,8 +52542,11 @@
       <c r="J87">
         <v>3248.15</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K87">
+        <v>2744.29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -51540,8 +52577,11 @@
       <c r="J88">
         <v>3288.24</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K88">
+        <v>2727.21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -51572,8 +52612,11 @@
       <c r="J89">
         <v>3313.54</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K89">
+        <v>2747.07</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -51604,8 +52647,11 @@
       <c r="J90">
         <v>3359.15</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K90">
+        <v>2787.43</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -51636,8 +52682,11 @@
       <c r="J91">
         <v>3374.85</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K91">
+        <v>2814.13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -51668,8 +52717,11 @@
       <c r="J92">
         <v>3387.12</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K92">
+        <v>2832.07</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -51700,8 +52752,11 @@
       <c r="J93">
         <v>3389.02</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K93">
+        <v>2845.69</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -51732,8 +52787,11 @@
       <c r="J94">
         <v>3378.8</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K94">
+        <v>2839.33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -51764,8 +52822,11 @@
       <c r="J95">
         <v>3344.89</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K95">
+        <v>2783.28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -51796,8 +52857,11 @@
       <c r="J96">
         <v>3316.24</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K96">
+        <v>2746.08</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -51828,8 +52892,11 @@
       <c r="J97">
         <v>3276.01</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K97">
+        <v>2729.64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -51860,8 +52927,11 @@
       <c r="J98">
         <v>3212.2</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K98">
+        <v>2691.61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -51892,8 +52962,11 @@
       <c r="J99">
         <v>3147.47</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K99">
+        <v>2640.92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -51924,8 +52997,11 @@
       <c r="J100">
         <v>3078.44</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K100">
+        <v>2559.92</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -51956,8 +53032,11 @@
       <c r="J101">
         <v>2999.06</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K101">
+        <v>2491.91</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -51988,8 +53067,11 @@
       <c r="J102">
         <v>2934.82</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K102">
+        <v>2445.04</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -52020,8 +53102,11 @@
       <c r="J103">
         <v>2864.59</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K103">
+        <v>2388.0500000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -52052,8 +53137,11 @@
       <c r="J104">
         <v>2799.81</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K104">
+        <v>2301.31</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -52084,8 +53172,11 @@
       <c r="J105">
         <v>2740.14</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K105">
+        <v>2248.7199999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -52116,8 +53207,11 @@
       <c r="J106">
         <v>2673.53</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K106">
+        <v>2143.19</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -52148,8 +53242,11 @@
       <c r="J107">
         <v>2615.4</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K107">
+        <v>2012.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -52180,8 +53277,11 @@
       <c r="J108">
         <v>2549.9299999999998</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K108">
+        <v>1892.85</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -52212,8 +53312,11 @@
       <c r="J109">
         <v>2495.19</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K109">
+        <v>1822.47</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -52244,8 +53347,11 @@
       <c r="J110">
         <v>2448.3000000000002</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K110">
+        <v>1863.41</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -52276,8 +53382,11 @@
       <c r="J111">
         <v>2404.09</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K111">
+        <v>1877.9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -52308,8 +53417,11 @@
       <c r="J112">
         <v>2364.1799999999998</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K112">
+        <v>1841.11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -52340,8 +53452,11 @@
       <c r="J113">
         <v>2318.86</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K113">
+        <v>1763.71</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -52372,8 +53487,11 @@
       <c r="J114">
         <v>2283.39</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K114">
+        <v>1698.81</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -52404,8 +53522,11 @@
       <c r="J115">
         <v>2238.19</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K115">
+        <v>1684.9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -52436,8 +53557,11 @@
       <c r="J116">
         <v>2204.27</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K116">
+        <v>1655.23</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -52468,8 +53592,11 @@
       <c r="J117">
         <v>2166.41</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K117">
+        <v>1619.13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -52500,8 +53627,11 @@
       <c r="J118">
         <v>2128.31</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K118">
+        <v>1586.02</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -52532,8 +53662,11 @@
       <c r="J119">
         <v>2087.5500000000002</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K119">
+        <v>1564.88</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -52564,8 +53697,11 @@
       <c r="J120">
         <v>2048.6999999999998</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K120">
+        <v>1536.53</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -52595,6 +53731,9 @@
       </c>
       <c r="J121">
         <v>2017.69</v>
+      </c>
+      <c r="K121">
+        <v>1548.89</v>
       </c>
     </row>
   </sheetData>
@@ -55411,7 +56550,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEDFA27-F7CC-45D4-A74F-72C1203A2D70}">
-  <dimension ref="A1:X121"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>

</xml_diff>

<commit_message>
Tweaked the fps test parameters so I don't have to wait for ages for a render to finish and made the warp locality graph title in the spreadsheet more descriptive.
</commit_message>
<xml_diff>
--- a/Statistics/BVH_Performance.xlsx
+++ b/Statistics/BVH_Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Projects\Radiance\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869BDBE3-6A05-433B-B3F4-7EDCECAE7A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F92BA17-4E48-4767-BA87-B0DAC65A5479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A5432B80-60C3-4BA9-AB2E-A1ED8FBAF94F}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>Warp locality 2 SPP</t>
   </si>
   <si>
-    <t>WL 2 SPP SbP offset</t>
-  </si>
-  <si>
     <t>Binned BVH</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Const BVH V2</t>
+  </si>
+  <si>
+    <t>Warp Locality 2 SPP SbP offset</t>
   </si>
 </sst>
 </file>
@@ -4812,7 +4812,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>WL 2 SPP SbP offset</c:v>
+                  <c:v>Warp Locality 2 SPP SbP offset</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7160,7 +7160,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$I$1</c15:sqref>
@@ -7191,7 +7191,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$A$2:$A$121</c15:sqref>
@@ -7566,7 +7566,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$I$2:$I$121</c15:sqref>
@@ -7940,7 +7940,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-C140-4A67-9C47-B4EB34F08BDB}"/>
                   </c:ext>
@@ -7953,7 +7953,7 @@
                 <c:order val="9"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$K$1</c15:sqref>
@@ -7984,7 +7984,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$A$2:$A$121</c15:sqref>
@@ -8359,7 +8359,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$K$2:$K$121</c15:sqref>
@@ -8733,7 +8733,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-E83C-41A1-A7BB-93C155C1481B}"/>
                   </c:ext>
@@ -8746,7 +8746,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$L$1</c15:sqref>
@@ -8777,7 +8777,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$A$2:$A$121</c15:sqref>
@@ -9152,7 +9152,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$L$2:$L$121</c15:sqref>
@@ -9526,7 +9526,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-97CD-4A7A-9F0E-261555781BC7}"/>
                   </c:ext>
@@ -14543,7 +14543,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>WL 2 SPP SbP offset</c:v>
+                  <c:v>Warp Locality 2 SPP SbP offset</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16891,7 +16891,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$I$124</c15:sqref>
@@ -16922,7 +16922,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$A$125:$A$244</c15:sqref>
@@ -17297,7 +17297,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$I$125:$I$244</c15:sqref>
@@ -17671,7 +17671,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-C57B-476E-B11C-2CCD19F91321}"/>
                   </c:ext>
@@ -17684,7 +17684,7 @@
                 <c:order val="9"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$K$124</c15:sqref>
@@ -17715,7 +17715,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$A$125:$A$244</c15:sqref>
@@ -18090,7 +18090,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$K$125:$K$244</c15:sqref>
@@ -18464,7 +18464,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-C57B-476E-B11C-2CCD19F91321}"/>
                   </c:ext>
@@ -18477,7 +18477,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$L$124</c15:sqref>
@@ -18508,7 +18508,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$A$125:$A$244</c15:sqref>
@@ -18883,7 +18883,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'unity.tri MSPS'!$L$125:$L$244</c15:sqref>
@@ -19257,7 +19257,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-C57B-476E-B11C-2CCD19F91321}"/>
                   </c:ext>
@@ -19437,7 +19437,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-GB"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -29054,8 +29054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8750E5EE-F956-401B-AB0D-294E07FBDD80}">
   <dimension ref="A1:M244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="E99" workbookViewId="0">
+      <selection activeCell="O106" sqref="O106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29069,7 +29069,7 @@
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29102,16 +29102,16 @@
         <v>15</v>
       </c>
       <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -34060,16 +34060,16 @@
         <v>15</v>
       </c>
       <c r="J124" t="s">
+        <v>19</v>
+      </c>
+      <c r="K124" t="s">
+        <v>17</v>
+      </c>
+      <c r="L124" t="s">
+        <v>18</v>
+      </c>
+      <c r="M124" t="s">
         <v>16</v>
-      </c>
-      <c r="K124" t="s">
-        <v>18</v>
-      </c>
-      <c r="L124" t="s">
-        <v>19</v>
-      </c>
-      <c r="M124" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>